<commit_message>
refactor: invoice import - not finished yet
</commit_message>
<xml_diff>
--- a/source/public/files/ChungTuNhapKhau.xlsx
+++ b/source/public/files/ChungTuNhapKhau.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Data\Laravel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ving\Desktop\IAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16589EE-164E-4850-9149-B0EFC70A7A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B923713B-28A0-4F87-8FE4-B56EFF6E8A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B27A79C-BAF0-4907-9BB7-CD247F375C40}"/>
   </bookViews>
@@ -297,21 +297,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -339,6 +324,21 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -359,9 +359,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -399,7 +399,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -505,7 +505,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -647,7 +647,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E4D763-AB37-4255-9781-62648E94CBDB}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
     <col min="16" max="18" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -735,87 +735,88 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7" t="s">
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8" t="s">
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
     </row>
-    <row r="4" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="10" t="s">
+    <row r="4" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="13" t="s">
+      <c r="P4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="Q4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -826,10 +827,10 @@
       <c r="B5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="9">
         <v>105467671150</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="13">
         <v>45068</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -838,16 +839,16 @@
       <c r="F5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="10" t="s">
         <v>39</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="11">
         <v>22032</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="12">
         <v>0.25</v>
       </c>
       <c r="K5" s="3" t="s">

</xml_diff>